<commit_message>
rapport + corrections antenne
</commit_message>
<xml_diff>
--- a/Rapport/planning.xlsx
+++ b/Rapport/planning.xlsx
@@ -2911,6 +2911,42 @@
     <xf numFmtId="0" fontId="24" fillId="5" borderId="10" xfId="37" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2918,45 +2954,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5394,8 +5394,8 @@
   <dimension ref="A1:CX40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5423,27 +5423,27 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="130"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
+      <c r="K1" s="174"/>
+      <c r="L1" s="174"/>
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174"/>
+      <c r="U1" s="174"/>
+      <c r="V1" s="174"/>
+      <c r="W1" s="174"/>
+      <c r="X1" s="174"/>
+      <c r="Y1" s="174"/>
+      <c r="Z1" s="174"/>
+      <c r="AA1" s="174"/>
+      <c r="AB1" s="174"/>
+      <c r="AC1" s="174"/>
+      <c r="AD1" s="174"/>
+      <c r="AE1" s="174"/>
     </row>
     <row r="2" spans="1:101" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
@@ -5488,11 +5488,11 @@
       <c r="B4" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="167">
+      <c r="C4" s="176">
         <v>43598</v>
       </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
       <c r="F4" s="110"/>
       <c r="G4" s="113" t="s">
         <v>73</v>
@@ -5502,282 +5502,282 @@
       </c>
       <c r="I4" s="111"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="164" t="str">
+      <c r="K4" s="168" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="165"/>
-      <c r="M4" s="165"/>
-      <c r="N4" s="165"/>
-      <c r="O4" s="165"/>
-      <c r="P4" s="165"/>
-      <c r="Q4" s="166"/>
-      <c r="R4" s="164" t="str">
+      <c r="L4" s="169"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="169"/>
+      <c r="O4" s="169"/>
+      <c r="P4" s="169"/>
+      <c r="Q4" s="170"/>
+      <c r="R4" s="168" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="165"/>
-      <c r="T4" s="165"/>
-      <c r="U4" s="165"/>
-      <c r="V4" s="165"/>
-      <c r="W4" s="165"/>
-      <c r="X4" s="166"/>
-      <c r="Y4" s="164" t="str">
+      <c r="S4" s="169"/>
+      <c r="T4" s="169"/>
+      <c r="U4" s="169"/>
+      <c r="V4" s="169"/>
+      <c r="W4" s="169"/>
+      <c r="X4" s="170"/>
+      <c r="Y4" s="168" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="165"/>
-      <c r="AA4" s="165"/>
-      <c r="AB4" s="165"/>
-      <c r="AC4" s="165"/>
-      <c r="AD4" s="165"/>
-      <c r="AE4" s="166"/>
-      <c r="AF4" s="164" t="str">
+      <c r="Z4" s="169"/>
+      <c r="AA4" s="169"/>
+      <c r="AB4" s="169"/>
+      <c r="AC4" s="169"/>
+      <c r="AD4" s="169"/>
+      <c r="AE4" s="170"/>
+      <c r="AF4" s="168" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="165"/>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="165"/>
-      <c r="AJ4" s="165"/>
-      <c r="AK4" s="165"/>
-      <c r="AL4" s="166"/>
-      <c r="AM4" s="164" t="str">
+      <c r="AG4" s="169"/>
+      <c r="AH4" s="169"/>
+      <c r="AI4" s="169"/>
+      <c r="AJ4" s="169"/>
+      <c r="AK4" s="169"/>
+      <c r="AL4" s="170"/>
+      <c r="AM4" s="168" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="165"/>
-      <c r="AO4" s="165"/>
-      <c r="AP4" s="165"/>
-      <c r="AQ4" s="165"/>
-      <c r="AR4" s="165"/>
-      <c r="AS4" s="166"/>
-      <c r="AT4" s="164" t="str">
+      <c r="AN4" s="169"/>
+      <c r="AO4" s="169"/>
+      <c r="AP4" s="169"/>
+      <c r="AQ4" s="169"/>
+      <c r="AR4" s="169"/>
+      <c r="AS4" s="170"/>
+      <c r="AT4" s="168" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="165"/>
-      <c r="AV4" s="165"/>
-      <c r="AW4" s="165"/>
-      <c r="AX4" s="165"/>
-      <c r="AY4" s="165"/>
-      <c r="AZ4" s="166"/>
-      <c r="BA4" s="164" t="str">
+      <c r="AU4" s="169"/>
+      <c r="AV4" s="169"/>
+      <c r="AW4" s="169"/>
+      <c r="AX4" s="169"/>
+      <c r="AY4" s="169"/>
+      <c r="AZ4" s="170"/>
+      <c r="BA4" s="168" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="165"/>
-      <c r="BC4" s="165"/>
-      <c r="BD4" s="165"/>
-      <c r="BE4" s="165"/>
-      <c r="BF4" s="165"/>
-      <c r="BG4" s="166"/>
-      <c r="BH4" s="164" t="str">
+      <c r="BB4" s="169"/>
+      <c r="BC4" s="169"/>
+      <c r="BD4" s="169"/>
+      <c r="BE4" s="169"/>
+      <c r="BF4" s="169"/>
+      <c r="BG4" s="170"/>
+      <c r="BH4" s="168" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="165"/>
-      <c r="BJ4" s="165"/>
-      <c r="BK4" s="165"/>
-      <c r="BL4" s="165"/>
-      <c r="BM4" s="165"/>
-      <c r="BN4" s="166"/>
-      <c r="BO4" s="171" t="str">
+      <c r="BI4" s="169"/>
+      <c r="BJ4" s="169"/>
+      <c r="BK4" s="169"/>
+      <c r="BL4" s="169"/>
+      <c r="BM4" s="169"/>
+      <c r="BN4" s="170"/>
+      <c r="BO4" s="162" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BP4" s="172"/>
-      <c r="BQ4" s="172"/>
-      <c r="BR4" s="172"/>
-      <c r="BS4" s="172"/>
-      <c r="BT4" s="172"/>
-      <c r="BU4" s="173"/>
-      <c r="BV4" s="171" t="str">
+      <c r="BP4" s="163"/>
+      <c r="BQ4" s="163"/>
+      <c r="BR4" s="163"/>
+      <c r="BS4" s="163"/>
+      <c r="BT4" s="163"/>
+      <c r="BU4" s="164"/>
+      <c r="BV4" s="162" t="str">
         <f>"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BW4" s="172"/>
-      <c r="BX4" s="172"/>
-      <c r="BY4" s="172"/>
-      <c r="BZ4" s="172"/>
-      <c r="CA4" s="172"/>
-      <c r="CB4" s="173"/>
-      <c r="CC4" s="171" t="str">
+      <c r="BW4" s="163"/>
+      <c r="BX4" s="163"/>
+      <c r="BY4" s="163"/>
+      <c r="BZ4" s="163"/>
+      <c r="CA4" s="163"/>
+      <c r="CB4" s="164"/>
+      <c r="CC4" s="162" t="str">
         <f>"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="CD4" s="172"/>
-      <c r="CE4" s="172"/>
-      <c r="CF4" s="172"/>
-      <c r="CG4" s="172"/>
-      <c r="CH4" s="172"/>
-      <c r="CI4" s="173"/>
-      <c r="CJ4" s="171" t="str">
+      <c r="CD4" s="163"/>
+      <c r="CE4" s="163"/>
+      <c r="CF4" s="163"/>
+      <c r="CG4" s="163"/>
+      <c r="CH4" s="163"/>
+      <c r="CI4" s="164"/>
+      <c r="CJ4" s="162" t="str">
         <f>"Week "&amp;(CJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="CK4" s="172"/>
-      <c r="CL4" s="172"/>
-      <c r="CM4" s="172"/>
-      <c r="CN4" s="172"/>
-      <c r="CO4" s="172"/>
-      <c r="CP4" s="173"/>
-      <c r="CQ4" s="171" t="str">
+      <c r="CK4" s="163"/>
+      <c r="CL4" s="163"/>
+      <c r="CM4" s="163"/>
+      <c r="CN4" s="163"/>
+      <c r="CO4" s="163"/>
+      <c r="CP4" s="164"/>
+      <c r="CQ4" s="162" t="str">
         <f>"Week "&amp;(CQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="CR4" s="172"/>
-      <c r="CS4" s="172"/>
-      <c r="CT4" s="172"/>
-      <c r="CU4" s="172"/>
-      <c r="CV4" s="172"/>
-      <c r="CW4" s="173"/>
+      <c r="CR4" s="163"/>
+      <c r="CS4" s="163"/>
+      <c r="CT4" s="163"/>
+      <c r="CU4" s="163"/>
+      <c r="CV4" s="163"/>
+      <c r="CW4" s="164"/>
     </row>
     <row r="5" spans="1:101" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="109"/>
       <c r="B5" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="163">
+      <c r="C5" s="175">
         <v>43693</v>
       </c>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
+      <c r="D5" s="175"/>
+      <c r="E5" s="175"/>
       <c r="F5" s="112"/>
       <c r="G5" s="112"/>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="168">
+      <c r="K5" s="171">
         <f>K6</f>
         <v>43598</v>
       </c>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="170"/>
-      <c r="R5" s="168">
+      <c r="L5" s="172"/>
+      <c r="M5" s="172"/>
+      <c r="N5" s="172"/>
+      <c r="O5" s="172"/>
+      <c r="P5" s="172"/>
+      <c r="Q5" s="173"/>
+      <c r="R5" s="171">
         <f>R6</f>
         <v>43605</v>
       </c>
-      <c r="S5" s="169"/>
-      <c r="T5" s="169"/>
-      <c r="U5" s="169"/>
-      <c r="V5" s="169"/>
-      <c r="W5" s="169"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="168">
+      <c r="S5" s="172"/>
+      <c r="T5" s="172"/>
+      <c r="U5" s="172"/>
+      <c r="V5" s="172"/>
+      <c r="W5" s="172"/>
+      <c r="X5" s="173"/>
+      <c r="Y5" s="171">
         <f>Y6</f>
         <v>43612</v>
       </c>
-      <c r="Z5" s="169"/>
-      <c r="AA5" s="169"/>
-      <c r="AB5" s="169"/>
-      <c r="AC5" s="169"/>
-      <c r="AD5" s="169"/>
-      <c r="AE5" s="170"/>
-      <c r="AF5" s="168">
+      <c r="Z5" s="172"/>
+      <c r="AA5" s="172"/>
+      <c r="AB5" s="172"/>
+      <c r="AC5" s="172"/>
+      <c r="AD5" s="172"/>
+      <c r="AE5" s="173"/>
+      <c r="AF5" s="171">
         <f>AF6</f>
         <v>43619</v>
       </c>
-      <c r="AG5" s="169"/>
-      <c r="AH5" s="169"/>
-      <c r="AI5" s="169"/>
-      <c r="AJ5" s="169"/>
-      <c r="AK5" s="169"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="168">
+      <c r="AG5" s="172"/>
+      <c r="AH5" s="172"/>
+      <c r="AI5" s="172"/>
+      <c r="AJ5" s="172"/>
+      <c r="AK5" s="172"/>
+      <c r="AL5" s="173"/>
+      <c r="AM5" s="171">
         <f>AM6</f>
         <v>43626</v>
       </c>
-      <c r="AN5" s="169"/>
-      <c r="AO5" s="169"/>
-      <c r="AP5" s="169"/>
-      <c r="AQ5" s="169"/>
-      <c r="AR5" s="169"/>
-      <c r="AS5" s="170"/>
-      <c r="AT5" s="168">
+      <c r="AN5" s="172"/>
+      <c r="AO5" s="172"/>
+      <c r="AP5" s="172"/>
+      <c r="AQ5" s="172"/>
+      <c r="AR5" s="172"/>
+      <c r="AS5" s="173"/>
+      <c r="AT5" s="171">
         <f>AT6</f>
         <v>43633</v>
       </c>
-      <c r="AU5" s="169"/>
-      <c r="AV5" s="169"/>
-      <c r="AW5" s="169"/>
-      <c r="AX5" s="169"/>
-      <c r="AY5" s="169"/>
-      <c r="AZ5" s="170"/>
-      <c r="BA5" s="168">
+      <c r="AU5" s="172"/>
+      <c r="AV5" s="172"/>
+      <c r="AW5" s="172"/>
+      <c r="AX5" s="172"/>
+      <c r="AY5" s="172"/>
+      <c r="AZ5" s="173"/>
+      <c r="BA5" s="171">
         <f>BA6</f>
         <v>43640</v>
       </c>
-      <c r="BB5" s="169"/>
-      <c r="BC5" s="169"/>
-      <c r="BD5" s="169"/>
-      <c r="BE5" s="169"/>
-      <c r="BF5" s="169"/>
-      <c r="BG5" s="170"/>
-      <c r="BH5" s="168">
+      <c r="BB5" s="172"/>
+      <c r="BC5" s="172"/>
+      <c r="BD5" s="172"/>
+      <c r="BE5" s="172"/>
+      <c r="BF5" s="172"/>
+      <c r="BG5" s="173"/>
+      <c r="BH5" s="171">
         <f>BH6</f>
         <v>43647</v>
       </c>
-      <c r="BI5" s="169"/>
-      <c r="BJ5" s="169"/>
-      <c r="BK5" s="169"/>
-      <c r="BL5" s="169"/>
-      <c r="BM5" s="169"/>
-      <c r="BN5" s="170"/>
-      <c r="BO5" s="174">
+      <c r="BI5" s="172"/>
+      <c r="BJ5" s="172"/>
+      <c r="BK5" s="172"/>
+      <c r="BL5" s="172"/>
+      <c r="BM5" s="172"/>
+      <c r="BN5" s="173"/>
+      <c r="BO5" s="165">
         <f>BO6</f>
         <v>43654</v>
       </c>
-      <c r="BP5" s="175"/>
-      <c r="BQ5" s="175"/>
-      <c r="BR5" s="175"/>
-      <c r="BS5" s="175"/>
-      <c r="BT5" s="175"/>
-      <c r="BU5" s="176"/>
-      <c r="BV5" s="174">
+      <c r="BP5" s="166"/>
+      <c r="BQ5" s="166"/>
+      <c r="BR5" s="166"/>
+      <c r="BS5" s="166"/>
+      <c r="BT5" s="166"/>
+      <c r="BU5" s="167"/>
+      <c r="BV5" s="165">
         <f>BV6</f>
         <v>43661</v>
       </c>
-      <c r="BW5" s="175"/>
-      <c r="BX5" s="175"/>
-      <c r="BY5" s="175"/>
-      <c r="BZ5" s="175"/>
-      <c r="CA5" s="175"/>
-      <c r="CB5" s="176"/>
-      <c r="CC5" s="174">
+      <c r="BW5" s="166"/>
+      <c r="BX5" s="166"/>
+      <c r="BY5" s="166"/>
+      <c r="BZ5" s="166"/>
+      <c r="CA5" s="166"/>
+      <c r="CB5" s="167"/>
+      <c r="CC5" s="165">
         <f>CC6</f>
         <v>43668</v>
       </c>
-      <c r="CD5" s="175"/>
-      <c r="CE5" s="175"/>
-      <c r="CF5" s="175"/>
-      <c r="CG5" s="175"/>
-      <c r="CH5" s="175"/>
-      <c r="CI5" s="176"/>
-      <c r="CJ5" s="174">
+      <c r="CD5" s="166"/>
+      <c r="CE5" s="166"/>
+      <c r="CF5" s="166"/>
+      <c r="CG5" s="166"/>
+      <c r="CH5" s="166"/>
+      <c r="CI5" s="167"/>
+      <c r="CJ5" s="165">
         <f>CJ6</f>
         <v>43675</v>
       </c>
-      <c r="CK5" s="175"/>
-      <c r="CL5" s="175"/>
-      <c r="CM5" s="175"/>
-      <c r="CN5" s="175"/>
-      <c r="CO5" s="175"/>
-      <c r="CP5" s="176"/>
-      <c r="CQ5" s="174">
+      <c r="CK5" s="166"/>
+      <c r="CL5" s="166"/>
+      <c r="CM5" s="166"/>
+      <c r="CN5" s="166"/>
+      <c r="CO5" s="166"/>
+      <c r="CP5" s="167"/>
+      <c r="CQ5" s="165">
         <f>CQ6</f>
         <v>43682</v>
       </c>
-      <c r="CR5" s="175"/>
-      <c r="CS5" s="175"/>
-      <c r="CT5" s="175"/>
-      <c r="CU5" s="175"/>
-      <c r="CV5" s="175"/>
-      <c r="CW5" s="176"/>
+      <c r="CR5" s="166"/>
+      <c r="CS5" s="166"/>
+      <c r="CT5" s="166"/>
+      <c r="CU5" s="166"/>
+      <c r="CV5" s="166"/>
+      <c r="CW5" s="167"/>
     </row>
     <row r="6" spans="1:101" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
@@ -6892,7 +6892,7 @@
         <v>89</v>
       </c>
       <c r="H11" s="63">
-        <v>7.0000000000000007E-2</v>
+        <v>0.09</v>
       </c>
       <c r="I11" s="64"/>
       <c r="J11" s="95"/>
@@ -7329,7 +7329,7 @@
         <v>5</v>
       </c>
       <c r="H15" s="63">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I15" s="64"/>
       <c r="J15" s="95"/>
@@ -7555,7 +7555,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="63">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I17" s="64"/>
       <c r="J17" s="95"/>
@@ -7897,10 +7897,10 @@
       </c>
       <c r="F20" s="101">
         <f t="shared" si="43"/>
-        <v>43632</v>
+        <v>43630</v>
       </c>
       <c r="G20" s="62">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H20" s="63">
         <v>0</v>
@@ -9794,12 +9794,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="29">
-    <mergeCell ref="CC4:CI4"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="CJ4:CP4"/>
-    <mergeCell ref="CJ5:CP5"/>
-    <mergeCell ref="CQ4:CW4"/>
-    <mergeCell ref="CQ5:CW5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="BO4:BU4"/>
     <mergeCell ref="BO5:BU5"/>
     <mergeCell ref="BV4:CB4"/>
@@ -9814,15 +9817,12 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="CJ4:CP4"/>
+    <mergeCell ref="CJ5:CP5"/>
+    <mergeCell ref="CQ4:CW4"/>
+    <mergeCell ref="CQ5:CW5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H10:H21 H8 H23:H27 H29:H38">

</xml_diff>